<commit_message>
template correcto de reporte flujo efectivo anual
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/flujoefectivoanual.xlsx
+++ b/public/application/files/jasper/templates/flujoefectivoanual.xlsx
@@ -170,9 +170,6 @@
     <t>{tot:pct}</t>
   </si>
   <si>
-    <t>{subcat:nombre}</t>
-  </si>
-  <si>
     <t>{sub:mes1}</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>{sub:pct}</t>
+  </si>
+  <si>
+    <t>{sub:nombre}</t>
   </si>
 </sst>
 </file>
@@ -355,18 +355,6 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -384,6 +372,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,325 +718,325 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:O14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:15" ht="29.75" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15" ht="29.75" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
     </row>
     <row r="3" spans="1:15" ht="28">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
     </row>
     <row r="4" spans="1:15" ht="22.25" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:15" ht="18">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:15" s="8" customFormat="1">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:15" s="4" customFormat="1">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="13" t="s">
+      <c r="M11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="N11" s="13" t="s">
+      <c r="N11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="O11" s="13" t="s">
+      <c r="O11" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="C14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="E14" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="F14" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="G14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="H14" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="I14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="K14" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="L14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="M14" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="N14" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="N14" s="15" t="s">
+      <c r="O14" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="O14" s="15" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reportes funcionando con ingresos y total ingresos en html o archivo
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/flujoefectivoanual.xlsx
+++ b/public/application/files/jasper/templates/flujoefectivoanual.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="14060" tabRatio="198"/>
+    <workbookView xWindow="-36980" yWindow="0" windowWidth="28880" windowHeight="16880" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t>{compania:nombre}</t>
   </si>
@@ -80,96 +80,9 @@
     <t>Total</t>
   </si>
   <si>
-    <t>{categoria:nombre}</t>
-  </si>
-  <si>
-    <t>{categoria:mes1}</t>
-  </si>
-  <si>
-    <t>{categoria:mes2}</t>
-  </si>
-  <si>
-    <t>{categoria:mes3}</t>
-  </si>
-  <si>
-    <t>{categoria:mes4}</t>
-  </si>
-  <si>
-    <t>{categoria:mes5}</t>
-  </si>
-  <si>
-    <t>{categoria:mes6}</t>
-  </si>
-  <si>
-    <t>{categoria:mes7}</t>
-  </si>
-  <si>
-    <t>{categoria:mes8}</t>
-  </si>
-  <si>
-    <t>{categoria:mes9}</t>
-  </si>
-  <si>
-    <t>{categoria:mes10}</t>
-  </si>
-  <si>
-    <t>{categoria:mes11}</t>
-  </si>
-  <si>
-    <t>{categoria:mes12}</t>
-  </si>
-  <si>
-    <t>{categoria:total}</t>
-  </si>
-  <si>
-    <t>{categoria:pct}</t>
-  </si>
-  <si>
     <t>TOTALES</t>
   </si>
   <si>
-    <t>{tot:mes1}</t>
-  </si>
-  <si>
-    <t>{tot:mes2}</t>
-  </si>
-  <si>
-    <t>{tot:mes3}</t>
-  </si>
-  <si>
-    <t>{tot:mes4}</t>
-  </si>
-  <si>
-    <t>{tot:mes5}</t>
-  </si>
-  <si>
-    <t>{tot:mes6}</t>
-  </si>
-  <si>
-    <t>{tot:mes7}</t>
-  </si>
-  <si>
-    <t>{tot:mes8}</t>
-  </si>
-  <si>
-    <t>{tot:mes9}</t>
-  </si>
-  <si>
-    <t>{tot:mes10}</t>
-  </si>
-  <si>
-    <t>{tot:mes11}</t>
-  </si>
-  <si>
-    <t>{tot:mes12}</t>
-  </si>
-  <si>
-    <t>{tot:total}</t>
-  </si>
-  <si>
-    <t>{tot:pct}</t>
-  </si>
-  <si>
     <t>{sub:mes1}</t>
   </si>
   <si>
@@ -212,14 +125,140 @@
     <t>{sub:pct}</t>
   </si>
   <si>
-    <t>{sub:nombre}</t>
+    <t>{subt:mes1}</t>
+  </si>
+  <si>
+    <t>{ingreso:nombre}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes1}</t>
+  </si>
+  <si>
+    <t>{ingreso:total}</t>
+  </si>
+  <si>
+    <t>{ingreso:pct}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes1}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes2}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes3}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes4}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes5}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes6}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes7}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes8}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes9}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes10}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes11}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes12}</t>
+  </si>
+  <si>
+    <t>{ingresot:total}</t>
+  </si>
+  <si>
+    <t>{ingresot:pct}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes2}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes3}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes4}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes5}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes6}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes7}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes8}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes9}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes10}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes11}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes12}</t>
+  </si>
+  <si>
+    <t>{subt:mes2}</t>
+  </si>
+  <si>
+    <t>{subt:mes3}</t>
+  </si>
+  <si>
+    <t>{subt:mes4}</t>
+  </si>
+  <si>
+    <t>{subt:mes5}</t>
+  </si>
+  <si>
+    <t>{subt:mes7}</t>
+  </si>
+  <si>
+    <t>{subt:mes6}</t>
+  </si>
+  <si>
+    <t>{subt:mes8}</t>
+  </si>
+  <si>
+    <t>{subt:mes9}</t>
+  </si>
+  <si>
+    <t>{subt:mes10}</t>
+  </si>
+  <si>
+    <t>{subt:mes11}</t>
+  </si>
+  <si>
+    <t>{subt:mes12}</t>
+  </si>
+  <si>
+    <t>{subt:total}</t>
+  </si>
+  <si>
+    <t>{subt:pct}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -270,6 +309,22 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -350,8 +405,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -385,7 +450,17 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:XFD17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -878,49 +953,49 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="5" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -942,49 +1017,49 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="8" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -993,51 +1068,94 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="A14" s="8"/>
       <c r="B14" s="11" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="N14" s="11" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>62</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15 16384:16384">
+      <c r="B17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="XFD17" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1050,6 +1168,7 @@
     <mergeCell ref="D5:O5"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Ajuste inventario, relacion entrada compras, xlsx de reporte anual
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/flujoefectivoanual.xlsx
+++ b/public/application/files/jasper/templates/flujoefectivoanual.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36980" yWindow="0" windowWidth="28880" windowHeight="16880" tabRatio="198"/>
+    <workbookView xWindow="-28320" yWindow="0" windowWidth="25020" windowHeight="16920" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>{compania:nombre}</t>
   </si>
@@ -125,96 +125,99 @@
     <t>{sub:pct}</t>
   </si>
   <si>
+    <t>{sub:nombre}</t>
+  </si>
+  <si>
+    <t>{ingreso:nombre}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes1}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes2}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes3}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes4}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes5}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes6}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes7}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes8}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes9}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes10}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes11}</t>
+  </si>
+  <si>
+    <t>{ingreso:mes12}</t>
+  </si>
+  <si>
+    <t>{ingreso:total}</t>
+  </si>
+  <si>
+    <t>{ingreso:pct}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes1}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes2}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes3}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes4}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes5}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes6}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes7}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes8}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes9}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes10}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes11}</t>
+  </si>
+  <si>
+    <t>{ingresot:mes12}</t>
+  </si>
+  <si>
+    <t>{ingresot:total}</t>
+  </si>
+  <si>
+    <t>{ingresot:pct}</t>
+  </si>
+  <si>
     <t>{subt:mes1}</t>
   </si>
   <si>
-    <t>{ingreso:nombre}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes1}</t>
-  </si>
-  <si>
-    <t>{ingreso:total}</t>
-  </si>
-  <si>
-    <t>{ingreso:pct}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes1}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes2}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes3}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes4}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes5}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes6}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes7}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes8}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes9}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes10}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes11}</t>
-  </si>
-  <si>
-    <t>{ingreso:mes12}</t>
-  </si>
-  <si>
-    <t>{ingresot:total}</t>
-  </si>
-  <si>
-    <t>{ingresot:pct}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes2}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes3}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes4}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes5}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes6}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes7}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes8}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes9}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes10}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes11}</t>
-  </si>
-  <si>
-    <t>{ingresot:mes12}</t>
-  </si>
-  <si>
     <t>{subt:mes2}</t>
   </si>
   <si>
@@ -227,10 +230,10 @@
     <t>{subt:mes5}</t>
   </si>
   <si>
+    <t>{subt:mes6}</t>
+  </si>
+  <si>
     <t>{subt:mes7}</t>
-  </si>
-  <si>
-    <t>{subt:mes6}</t>
   </si>
   <si>
     <t>{subt:mes8}</t>
@@ -258,7 +261,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -312,22 +315,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -337,18 +324,9 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -393,74 +371,43 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="11">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -790,119 +737,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD17"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:15" ht="29.75" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
     </row>
     <row r="2" spans="1:15" ht="29.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
     </row>
     <row r="3" spans="1:15" ht="28">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
     </row>
     <row r="4" spans="1:15" ht="22.25" customHeight="1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
     </row>
     <row r="5" spans="1:15" ht="18">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:15" s="4" customFormat="1">
       <c r="A7" s="1" t="s">
@@ -952,210 +899,197 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="G8" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="H8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="I8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="J8" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="K8" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="L8" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="M8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="N8" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="O8" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>52</v>
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="8"/>
-      <c r="B14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="O14" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15 16384:16384">
-      <c r="B17" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="A13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="E13" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="F13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" s="11" t="s">
+      <c r="H13" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="I13" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="J13" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="K13" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="L13" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="M13" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="O17" s="11" t="s">
+      <c r="N13" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="XFD17" s="11"/>
+      <c r="O13" s="12" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1168,7 +1102,6 @@
     <mergeCell ref="D5:O5"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>